<commit_message>
refactor: update connection strings in appsettings.json and remove unused Resource.resx file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,20 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\notobo\source\repos\RecruitmentApp\RecruitmentApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\C#\ASP.NET\source\repos\RecruitmentApp\RecruitmentApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62B1653-2D42-4FCD-830E-8AB9A8B80C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F643B7-F756-4A99-8882-06D8BE02A47F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="company" sheetId="1" r:id="rId1"/>
-    <sheet name="Post" sheetId="3" r:id="rId2"/>
-    <sheet name="Address" sheetId="2" r:id="rId3"/>
-    <sheet name="Title" sheetId="4" r:id="rId4"/>
-    <sheet name="Levels" sheetId="5" r:id="rId5"/>
-    <sheet name="Skill" sheetId="6" r:id="rId6"/>
+    <sheet name="Images" sheetId="7" r:id="rId2"/>
+    <sheet name="Post" sheetId="3" r:id="rId3"/>
+    <sheet name="Address" sheetId="2" r:id="rId4"/>
+    <sheet name="Title" sheetId="4" r:id="rId5"/>
+    <sheet name="Levels" sheetId="5" r:id="rId6"/>
+    <sheet name="Skill" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="355">
   <si>
     <t>company_id</t>
   </si>
@@ -1053,6 +1054,54 @@
   </si>
   <si>
     <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>techombank.png</t>
+  </si>
+  <si>
+    <t>nab-innovation-centre-vietnam-14.jpg</t>
+  </si>
+  <si>
+    <t>sungrove-tech-viet-nam-13.jpg</t>
+  </si>
+  <si>
+    <t>cong-ty-tnhh-cong-nghe-asilla-viet-nam-11.jpg</t>
+  </si>
+  <si>
+    <t>ngan-hang-thuong-mai-co-phan-phat-trien-thanh-pho-ho-chi-minh-10.jpg</t>
+  </si>
+  <si>
+    <t>Asia.jpg</t>
+  </si>
+  <si>
+    <t>Scandinavian softwave park.png</t>
+  </si>
+  <si>
+    <t>nano-technologies-12.png</t>
+  </si>
+  <si>
+    <t>dich-vu-cong-nghe-ryte-viet-nam-16.png</t>
+  </si>
+  <si>
+    <t>ntt-data-vds-5.jpg</t>
+  </si>
+  <si>
+    <t>cong-ty-tnhh-isb-viet-nam-7.png</t>
+  </si>
+  <si>
+    <t>cong-ty-phan-mem-tower-hanoitohsoft-4.png</t>
+  </si>
+  <si>
+    <t>maple-labs-3.png</t>
+  </si>
+  <si>
+    <t>cong-ty-co-phan-chung-khoan-ky-thuong-techcom-securities-tcbs-17.png</t>
+  </si>
+  <si>
+    <t>nha-cung-cap-dich-vu-so-dsp-digital-service-provider-2.png</t>
+  </si>
+  <si>
+    <t>cong-ty-co-phan-propertyguru-viet-nam-8.png</t>
   </si>
 </sst>
 </file>
@@ -1210,7 +1259,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1269,6 +1318,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1487,24 +1545,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O999"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="68.109375" customWidth="1"/>
-    <col min="3" max="3" width="24.109375" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="42.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
     <col min="5" max="5" width="14.88671875" customWidth="1"/>
     <col min="6" max="6" width="19.44140625" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
     <col min="8" max="8" width="21.5546875" customWidth="1"/>
     <col min="9" max="9" width="17.33203125" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="54.109375" customWidth="1"/>
-    <col min="12" max="12" width="46.5546875" customWidth="1"/>
+    <col min="11" max="11" width="26.109375" customWidth="1"/>
+    <col min="12" max="12" width="21.5546875" customWidth="1"/>
     <col min="13" max="13" width="22.109375" customWidth="1"/>
     <col min="14" max="14" width="13.44140625" style="33" customWidth="1"/>
     <col min="15" max="15" width="18.77734375" customWidth="1"/>
@@ -1562,7 +1620,7 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1602,7 +1660,7 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="37" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1624,7 +1682,9 @@
         <v>17</v>
       </c>
       <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>339</v>
+      </c>
       <c r="K3" s="31" t="s">
         <v>24</v>
       </c>
@@ -1642,7 +1702,7 @@
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="37" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1664,7 +1724,9 @@
         <v>17</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>340</v>
+      </c>
       <c r="K4" s="2"/>
       <c r="L4" s="31" t="s">
         <v>32</v>
@@ -1680,7 +1742,7 @@
       <c r="A5" s="20">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="38" t="s">
         <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1702,7 +1764,9 @@
         <v>17</v>
       </c>
       <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>341</v>
+      </c>
       <c r="K5" s="31" t="s">
         <v>37</v>
       </c>
@@ -1718,7 +1782,7 @@
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="39" t="s">
         <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1740,7 +1804,9 @@
         <v>17</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="J6" t="s">
+        <v>346</v>
+      </c>
       <c r="K6" s="31" t="s">
         <v>43</v>
       </c>
@@ -1758,7 +1824,7 @@
       <c r="A7" s="20">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="37" t="s">
         <v>46</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1780,7 +1846,9 @@
         <v>17</v>
       </c>
       <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>342</v>
+      </c>
       <c r="K7" s="31" t="s">
         <v>48</v>
       </c>
@@ -1798,7 +1866,7 @@
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="40" t="s">
         <v>50</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1820,7 +1888,9 @@
         <v>17</v>
       </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>343</v>
+      </c>
       <c r="K8" s="31" t="s">
         <v>52</v>
       </c>
@@ -1838,7 +1908,7 @@
       <c r="A9" s="20">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="37" t="s">
         <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1860,7 +1930,9 @@
         <v>17</v>
       </c>
       <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="J9" s="2" t="s">
+        <v>347</v>
+      </c>
       <c r="K9" s="31" t="s">
         <v>59</v>
       </c>
@@ -1878,7 +1950,7 @@
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="37" t="s">
         <v>62</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -1900,7 +1972,9 @@
         <v>17</v>
       </c>
       <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="J10" s="2" t="s">
+        <v>345</v>
+      </c>
       <c r="K10" s="31" t="s">
         <v>65</v>
       </c>
@@ -1918,7 +1992,7 @@
       <c r="A11" s="20">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="37" t="s">
         <v>68</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1940,7 +2014,9 @@
         <v>17</v>
       </c>
       <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="J11" s="2" t="s">
+        <v>349</v>
+      </c>
       <c r="K11" s="31" t="s">
         <v>71</v>
       </c>
@@ -1958,7 +2034,7 @@
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="39" t="s">
         <v>74</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1980,7 +2056,9 @@
         <v>17</v>
       </c>
       <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="J12" s="2" t="s">
+        <v>344</v>
+      </c>
       <c r="K12" s="31" t="s">
         <v>77</v>
       </c>
@@ -1998,7 +2076,7 @@
       <c r="A13" s="20">
         <v>12</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="39" t="s">
         <v>80</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -2020,7 +2098,9 @@
         <v>17</v>
       </c>
       <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="J13" s="2" t="s">
+        <v>348</v>
+      </c>
       <c r="K13" s="31" t="s">
         <v>84</v>
       </c>
@@ -2036,7 +2116,7 @@
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="37" t="s">
         <v>86</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -2058,7 +2138,9 @@
         <v>17</v>
       </c>
       <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="J14" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="K14" s="31" t="s">
         <v>88</v>
       </c>
@@ -2076,7 +2158,7 @@
       <c r="A15" s="20">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="37" t="s">
         <v>90</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -2098,7 +2180,9 @@
         <v>17</v>
       </c>
       <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="J15" s="2" t="s">
+        <v>351</v>
+      </c>
       <c r="K15" s="31" t="s">
         <v>91</v>
       </c>
@@ -2116,7 +2200,7 @@
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -2138,7 +2222,9 @@
         <v>17</v>
       </c>
       <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="J16" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="K16" s="31" t="s">
         <v>96</v>
       </c>
@@ -2156,7 +2242,7 @@
       <c r="A17" s="20">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="37" t="s">
         <v>99</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -2178,7 +2264,9 @@
         <v>17</v>
       </c>
       <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="J17" s="2" t="s">
+        <v>354</v>
+      </c>
       <c r="K17" s="31" t="s">
         <v>102</v>
       </c>
@@ -2196,7 +2284,7 @@
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="39" t="s">
         <v>106</v>
       </c>
       <c r="C18" s="13" t="s">
@@ -2216,6 +2304,9 @@
       </c>
       <c r="H18" s="13" t="s">
         <v>108</v>
+      </c>
+      <c r="J18" t="s">
+        <v>352</v>
       </c>
       <c r="K18" s="31" t="s">
         <v>24</v>
@@ -3223,11 +3314,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C94B465-AE67-4135-A2D1-3679DC12E1FA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -4702,7 +4805,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -5182,7 +5285,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A1000"/>
   <sheetViews>
@@ -6348,7 +6451,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A1000"/>
   <sheetViews>
@@ -7393,7 +7496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>

</xml_diff>